<commit_message>
done 2 co pdf
</commit_message>
<xml_diff>
--- a/thong_so_bai_tap_lon.xlsx
+++ b/thong_so_bai_tap_lon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\nam3hk1\big-machine-elements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D0CCBE-FAFF-47F3-AF00-70F8D889D86C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC07CB72-EDCA-425E-870C-CECED7C3BD77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="5412" windowWidth="23256" windowHeight="12456" xr2:uid="{29AA01DD-013E-4F29-8126-57E0BCB14526}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Ka</t>
   </si>
@@ -69,6 +69,15 @@
   </si>
   <si>
     <t>zm</t>
+  </si>
+  <si>
+    <t>atw=at</t>
+  </si>
+  <si>
+    <t>beta b</t>
+  </si>
+  <si>
+    <t>bw</t>
   </si>
 </sst>
 </file>
@@ -440,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{467AC242-5BAC-41A8-B289-6103A445E493}">
-  <dimension ref="H8:I17"/>
+  <dimension ref="H8:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,31 +460,49 @@
     <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H8" t="s">
         <v>0</v>
       </c>
       <c r="I8">
         <v>43</v>
       </c>
-    </row>
-    <row r="9" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="L8" t="s">
+        <v>11</v>
+      </c>
+      <c r="M8">
+        <v>21.12</v>
+      </c>
+    </row>
+    <row r="9" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H9" t="s">
         <v>1</v>
       </c>
       <c r="I9">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="10" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="L9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M9">
+        <v>18.37</v>
+      </c>
+    </row>
+    <row r="10" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H10" t="s">
         <v>2</v>
       </c>
       <c r="I10">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="11" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="L10" t="s">
+        <v>13</v>
+      </c>
+      <c r="M10">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H11" t="s">
         <v>3</v>
       </c>
@@ -483,7 +510,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H12" t="s">
         <v>4</v>
       </c>
@@ -491,7 +518,7 @@
         <v>43.54</v>
       </c>
     </row>
-    <row r="13" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H13" t="s">
         <v>5</v>
       </c>
@@ -499,7 +526,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H14" t="s">
         <v>6</v>
       </c>
@@ -507,7 +534,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H15" t="s">
         <v>7</v>
       </c>
@@ -515,7 +542,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H16" t="s">
         <v>8</v>
       </c>

</xml_diff>